<commit_message>
KPMG releated folder added
</commit_message>
<xml_diff>
--- a/PEG Schedule.xlsx
+++ b/PEG Schedule.xlsx
@@ -4,19 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
   <si>
     <t>Start</t>
   </si>
@@ -70,9 +68,6 @@
   </si>
   <si>
     <t>After IR-1 Audit of Revised QMS</t>
-  </si>
-  <si>
-    <t>Activity</t>
   </si>
   <si>
     <t>Planned End</t>
@@ -129,9 +124,6 @@
   </si>
   <si>
     <t>14.0-17.30</t>
-  </si>
-  <si>
-    <t>16.45-18.00</t>
   </si>
   <si>
     <t>10.0-13.15
@@ -179,6 +171,31 @@
   </si>
   <si>
     <t>11-13.00  (Consolidated sheet completed)</t>
+  </si>
+  <si>
+    <t>16.30-17.30
+18.0-18.15</t>
+  </si>
+  <si>
+    <t>16.45-18.00 (Reviewed all changes and completed implementation.)</t>
+  </si>
+  <si>
+    <t>10.00-11.00</t>
+  </si>
+  <si>
+    <t>14.00-15.00</t>
+  </si>
+  <si>
+    <t>9.00-9.25</t>
+  </si>
+  <si>
+    <t>11.00-12.15</t>
+  </si>
+  <si>
+    <t>16.00-16.25</t>
+  </si>
+  <si>
+    <t>10.00-10.25</t>
   </si>
 </sst>
 </file>
@@ -249,10 +266,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -556,350 +573,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="9.140625" style="1"/>
-    <col min="12" max="12" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="3">
-        <v>44652</v>
-      </c>
-      <c r="H1" s="3">
-        <v>44653</v>
-      </c>
-      <c r="I1" s="3">
-        <v>44654</v>
-      </c>
-      <c r="J1" s="3">
-        <v>44655</v>
-      </c>
-      <c r="K1" s="3">
-        <v>44656</v>
-      </c>
-      <c r="L1" s="3">
-        <v>44657</v>
-      </c>
-      <c r="M1" s="3">
-        <v>44658</v>
-      </c>
-      <c r="N1" s="3">
-        <v>44660</v>
-      </c>
-    </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>44652</v>
-      </c>
-      <c r="D2" s="4">
-        <v>44652</v>
-      </c>
-      <c r="E2" s="4">
-        <v>44652</v>
-      </c>
-      <c r="F2" s="4">
-        <v>44652</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4">
-        <v>44652</v>
-      </c>
-      <c r="D3" s="4">
-        <v>44658</v>
-      </c>
-      <c r="E3" s="4">
-        <v>44652</v>
-      </c>
-      <c r="F3" s="4">
-        <v>44657</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4">
-        <v>44658</v>
-      </c>
-      <c r="D4" s="4">
-        <v>44676</v>
-      </c>
-      <c r="E4" s="4">
-        <v>44660</v>
-      </c>
-      <c r="F4" s="4">
-        <v>44669</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="4">
-        <v>44670</v>
-      </c>
-      <c r="D5" s="4">
-        <v>44672</v>
-      </c>
-      <c r="E5" s="4">
-        <v>44665</v>
-      </c>
-      <c r="F5" s="4">
-        <v>44672</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4">
-        <v>44676</v>
-      </c>
-      <c r="D6" s="4">
-        <v>44687</v>
-      </c>
-      <c r="E6" s="4">
-        <v>44669</v>
-      </c>
-      <c r="F6" s="4">
-        <v>44688</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="4">
-        <v>44687</v>
-      </c>
-      <c r="D7" s="4">
-        <v>44690</v>
-      </c>
-      <c r="E7" s="4">
-        <v>44690</v>
-      </c>
-      <c r="F7" s="4">
-        <v>44690</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="4">
-        <v>44690</v>
-      </c>
-      <c r="D8" s="4">
-        <v>44691</v>
-      </c>
-      <c r="E8" s="4">
-        <v>44691</v>
-      </c>
-      <c r="F8" s="4">
-        <v>44691</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="4">
-        <v>44691</v>
-      </c>
-      <c r="D9" s="4">
-        <v>44693</v>
-      </c>
-      <c r="E9" s="4">
-        <v>44691</v>
-      </c>
-      <c r="F9" s="4">
-        <v>44692</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4">
-        <v>44694</v>
-      </c>
-      <c r="E10" s="4">
-        <v>44697</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="4">
-        <v>44694</v>
-      </c>
-      <c r="E11" s="4">
-        <v>44694</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="4">
-        <v>44728</v>
-      </c>
-      <c r="D12" s="4">
-        <v>44734</v>
-      </c>
-      <c r="E12" s="4">
-        <v>44708</v>
-      </c>
-      <c r="F12" s="4">
-        <v>44755</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="4">
-        <v>44728</v>
-      </c>
-      <c r="D13" s="4">
-        <v>44734</v>
-      </c>
-      <c r="E13" s="4">
-        <v>44735</v>
-      </c>
-      <c r="F13" s="4">
-        <v>44753</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="4">
-        <v>44748</v>
-      </c>
-      <c r="D14" s="4">
-        <v>44750</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="4">
-        <v>44750</v>
-      </c>
-      <c r="D15" s="4">
-        <v>44751</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="4">
-        <v>44765</v>
-      </c>
-      <c r="D16" s="4">
-        <v>44768</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="4">
-        <v>44768</v>
-      </c>
-      <c r="D17" s="4">
-        <v>44776</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="4">
-        <v>44776</v>
-      </c>
-      <c r="D18" s="4">
-        <v>44785</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="4">
-        <v>44785</v>
-      </c>
-      <c r="D19" s="4">
-        <v>44786</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+      <selection pane="bottomLeft" activeCell="M107" sqref="M107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -971,7 +649,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="4">
         <v>44652</v>
@@ -1030,7 +708,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="4">
         <v>44652</v>
@@ -1085,7 +763,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4">
         <v>44652</v>
@@ -1118,10 +796,10 @@
         <v>44698</v>
       </c>
       <c r="L4" s="4">
-        <v>44708</v>
+        <v>44709</v>
       </c>
       <c r="M4" s="4">
-        <v>44735</v>
+        <v>44736</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -1132,7 +810,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4">
         <v>44652</v>
@@ -1161,7 +839,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="4">
-        <v>44755</v>
+        <v>44757</v>
       </c>
       <c r="M5" s="4">
         <v>44753</v>
@@ -1178,10 +856,10 @@
         <v>44652</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1198,8 +876,8 @@
       <c r="A9" s="3">
         <v>44655</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>24</v>
+      <c r="C9" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1211,8 +889,8 @@
       <c r="A11" s="3">
         <v>44657</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>26</v>
+      <c r="C11" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1229,8 +907,8 @@
       <c r="A14" s="3">
         <v>44660</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>27</v>
+      <c r="D14" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1242,35 +920,35 @@
       <c r="A16" s="3">
         <v>44662</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>28</v>
+      <c r="D16" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>44663</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>29</v>
+      <c r="D17" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>44664</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>30</v>
+      <c r="D18" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="84" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>44665</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>50</v>
+      <c r="D19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1292,14 +970,14 @@
       <c r="A23" s="3">
         <v>44669</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>48</v>
+      <c r="E23" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1311,16 +989,16 @@
       <c r="A25" s="3">
         <v>44671</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>47</v>
+      <c r="F25" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>44672</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>46</v>
+      <c r="F26" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1332,8 +1010,8 @@
       <c r="A28" s="3">
         <v>44674</v>
       </c>
-      <c r="F28" s="7" t="s">
-        <v>32</v>
+      <c r="F28" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1345,8 +1023,8 @@
       <c r="A30" s="3">
         <v>44676</v>
       </c>
-      <c r="F30" s="7" t="s">
-        <v>33</v>
+      <c r="F30" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1368,16 +1046,16 @@
       <c r="A34" s="3">
         <v>44680</v>
       </c>
-      <c r="F34" s="7" t="s">
-        <v>34</v>
+      <c r="F34" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>44681</v>
       </c>
-      <c r="F35" s="7" t="s">
-        <v>35</v>
+      <c r="F35" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1409,16 +1087,16 @@
       <c r="A41" s="3">
         <v>44687</v>
       </c>
-      <c r="F41" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F41" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>44688</v>
       </c>
-      <c r="F42" s="5" t="s">
-        <v>37</v>
+      <c r="F42" s="6" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -1430,27 +1108,27 @@
       <c r="A44" s="3">
         <v>44690</v>
       </c>
-      <c r="G44" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>39</v>
+      <c r="G44" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44691</v>
       </c>
-      <c r="I45" s="7" t="s">
-        <v>40</v>
+      <c r="I45" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>44692</v>
       </c>
-      <c r="I46" s="7" t="s">
-        <v>41</v>
+      <c r="I46" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -1463,340 +1141,361 @@
         <v>44694</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>44695</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>44696</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="24" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>44697</v>
       </c>
-      <c r="J51" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="J51" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="24" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>44698</v>
       </c>
-      <c r="K52" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K52" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>44699</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>44700</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>44701</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>44702</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>44703</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>44704</v>
       </c>
-      <c r="J58" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J58" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>44705</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>44706</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>44707</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>44708</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="24" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>44709</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L63" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>44710</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>44711</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>44712</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>44713</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>44714</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>44715</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="24" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>44716</v>
       </c>
-      <c r="K70" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K70" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>44717</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="24" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>44718</v>
       </c>
-      <c r="J72" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J72" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L72" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>44719</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>44720</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>44721</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>44722</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>44723</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>44724</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>44725</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>44726</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>44727</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>44728</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>44729</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>44730</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>44731</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>44732</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>44733</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>44734</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>44735</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" ht="24" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>44736</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M90" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>44737</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>44738</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" ht="24" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>44739</v>
       </c>
-      <c r="J93" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J93" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>44740</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>44741</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>44742</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>44743</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" ht="48" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>44744</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="N98" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>44745</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>44746</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>44747</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>44748</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>44749</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>44750</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>44751</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>44752</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>44753</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="M107" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>44754</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>44755</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L109" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>44756</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>44757</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L111" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>44758</v>
       </c>
@@ -1824,18 +1523,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>